<commit_message>
Waste Report Database Query Updated
</commit_message>
<xml_diff>
--- a/CCICertificate/WebContent/resources/in/WasteReport.xlsx
+++ b/CCICertificate/WebContent/resources/in/WasteReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>№</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Код ТН ВЭД</t>
+  </si>
+  <si>
+    <t>Регистрационный номер призводителя</t>
+  </si>
+  <si>
+    <t>Сесто нахождения призводителя</t>
+  </si>
+  <si>
+    <t>Наитменование товара</t>
   </si>
 </sst>
 </file>
@@ -94,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -165,11 +174,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -183,18 +201,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -204,6 +219,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -533,77 +555,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="32" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:7" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="1" t="s">
+    <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="J3" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="10">
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
WasteReport update. Added TNVED exceptions.
</commit_message>
<xml_diff>
--- a/CCICertificate/WebContent/resources/in/WasteReport.xlsx
+++ b/CCICertificate/WebContent/resources/in/WasteReport.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -43,9 +42,6 @@
     <t>Код ТН ВЭД</t>
   </si>
   <si>
-    <t>Регистрационный номер призводителя</t>
-  </si>
-  <si>
     <t>Дата выдачи сертификата</t>
   </si>
   <si>
@@ -53,6 +49,9 @@
   </si>
   <si>
     <t>Место нахождения (адрес) призводителя</t>
+  </si>
+  <si>
+    <t>УНП</t>
   </si>
 </sst>
 </file>
@@ -559,7 +558,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,13 +600,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>5</v>
@@ -617,7 +616,7 @@
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>